<commit_message>
split etl and prepare
</commit_message>
<xml_diff>
--- a/DATAMODEL_m5.xlsx
+++ b/DATAMODEL_m5.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2FCD35-9D1B-4BFB-9317-B214CD05B09E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="2375" windowWidth="21377" windowHeight="11268" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2928" yWindow="2376" windowWidth="21372" windowHeight="11268"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -13,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$F$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$F$85</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="145">
   <si>
     <t>table</t>
   </si>
@@ -254,9 +253,6 @@
     <t>if demand&gt;0</t>
   </si>
   <si>
-    <t>take care of missing prices</t>
-  </si>
-  <si>
     <t>demand_median</t>
   </si>
   <si>
@@ -358,9 +354,6 @@
     <t>snap_avg1week</t>
   </si>
   <si>
-    <t>price_ratio_to_90d_rolling</t>
-  </si>
-  <si>
     <t>maybe</t>
   </si>
   <si>
@@ -458,12 +451,18 @@
   </si>
   <si>
     <t>snap_avg2week</t>
+  </si>
+  <si>
+    <t>take care of missing prices, i.e. remove</t>
+  </si>
+  <si>
+    <t>price_ratio_to_8week_rolling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -576,6 +575,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -631,9 +633,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -671,9 +673,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -706,26 +708,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -758,26 +743,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -950,27 +918,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:XFD70"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1"/>
-    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="2" width="10.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1"/>
+    <col min="5" max="5" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.33203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +978,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
@@ -1030,7 +998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
@@ -1050,7 +1018,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
@@ -1070,7 +1038,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
@@ -1090,7 +1058,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
@@ -1110,7 +1078,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1130,7 +1098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -1148,7 +1116,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
@@ -1168,7 +1136,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1188,7 +1156,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>49</v>
       </c>
@@ -1205,10 +1173,10 @@
         <v>45</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -1228,7 +1196,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>49</v>
       </c>
@@ -1245,10 +1213,10 @@
         <v>56</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
@@ -1265,10 +1233,10 @@
         <v>45</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
@@ -1301,10 +1269,10 @@
         <v>61</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -1341,10 +1309,10 @@
         <v>62</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
@@ -1364,7 +1332,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>49</v>
       </c>
@@ -1381,10 +1349,10 @@
         <v>8</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
@@ -1404,7 +1372,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>49</v>
       </c>
@@ -1424,7 +1392,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>67</v>
       </c>
@@ -1440,7 +1408,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>67</v>
       </c>
@@ -1456,7 +1424,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>67</v>
       </c>
@@ -1472,7 +1440,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>67</v>
       </c>
@@ -1490,7 +1458,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
@@ -1508,7 +1476,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>7</v>
       </c>
@@ -1516,17 +1484,17 @@
         <v>22</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>7</v>
       </c>
@@ -1534,17 +1502,17 @@
         <v>22</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>7</v>
       </c>
@@ -1562,7 +1530,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>7</v>
       </c>
@@ -1580,7 +1548,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>7</v>
       </c>
@@ -1595,10 +1563,10 @@
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>7</v>
       </c>
@@ -1606,7 +1574,7 @@
         <v>22</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>28</v>
@@ -1615,10 +1583,10 @@
         <v>8</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>7</v>
       </c>
@@ -1626,7 +1594,7 @@
         <v>22</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>28</v>
@@ -1635,10 +1603,10 @@
         <v>61</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>7</v>
       </c>
@@ -1646,7 +1614,7 @@
         <v>22</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>28</v>
@@ -1655,10 +1623,10 @@
         <v>62</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>7</v>
       </c>
@@ -1666,7 +1634,7 @@
         <v>22</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>28</v>
@@ -1675,10 +1643,10 @@
         <v>8</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
@@ -1686,7 +1654,7 @@
         <v>22</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>28</v>
@@ -1696,7 +1664,7 @@
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>7</v>
       </c>
@@ -1704,7 +1672,7 @@
         <v>22</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>28</v>
@@ -1714,7 +1682,7 @@
       </c>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1690,7 @@
         <v>22</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>4</v>
@@ -1730,7 +1698,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>7</v>
       </c>
@@ -1738,7 +1706,7 @@
         <v>22</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>4</v>
@@ -1754,7 +1722,7 @@
         <v>22</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>28</v>
@@ -1763,10 +1731,10 @@
         <v>47</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>7</v>
       </c>
@@ -1774,7 +1742,7 @@
         <v>22</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>28</v>
@@ -1783,10 +1751,10 @@
         <v>8</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>7</v>
       </c>
@@ -1794,7 +1762,7 @@
         <v>22</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>28</v>
@@ -1804,7 +1772,7 @@
       </c>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>7</v>
       </c>
@@ -1812,7 +1780,7 @@
         <v>22</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>28</v>
@@ -1822,7 +1790,7 @@
       </c>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1798,7 @@
         <v>22</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>4</v>
@@ -1838,7 +1806,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>7</v>
       </c>
@@ -1846,7 +1814,7 @@
         <v>22</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>4</v>
@@ -1854,7 +1822,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>7</v>
       </c>
@@ -1872,7 +1840,7 @@
       </c>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +1858,7 @@
       </c>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>7</v>
       </c>
@@ -1906,7 +1874,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>7</v>
       </c>
@@ -1922,7 +1890,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>7</v>
       </c>
@@ -1938,7 +1906,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>7</v>
       </c>
@@ -1956,7 +1924,7 @@
       </c>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>7</v>
       </c>
@@ -1974,7 +1942,7 @@
       </c>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>7</v>
       </c>
@@ -1982,7 +1950,7 @@
         <v>22</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>4</v>
@@ -1990,7 +1958,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="5"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>7</v>
       </c>
@@ -1998,7 +1966,7 @@
         <v>22</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>4</v>
@@ -2006,7 +1974,7 @@
       <c r="E56" s="6"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>7</v>
       </c>
@@ -2014,7 +1982,7 @@
         <v>22</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>4</v>
@@ -2022,7 +1990,7 @@
       <c r="E57" s="6"/>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>7</v>
       </c>
@@ -2030,7 +1998,7 @@
         <v>22</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>4</v>
@@ -2038,7 +2006,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="5"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>7</v>
       </c>
@@ -2046,7 +2014,7 @@
         <v>22</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>4</v>
@@ -2054,7 +2022,7 @@
       <c r="E59" s="6"/>
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>7</v>
       </c>
@@ -2062,7 +2030,7 @@
         <v>22</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>4</v>
@@ -2070,7 +2038,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="5"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>7</v>
       </c>
@@ -2078,7 +2046,7 @@
         <v>22</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>4</v>
@@ -2086,7 +2054,7 @@
       <c r="E61" s="6"/>
       <c r="F61" s="5"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>7</v>
       </c>
@@ -2094,7 +2062,7 @@
         <v>22</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>28</v>
@@ -2102,7 +2070,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>7</v>
       </c>
@@ -2110,7 +2078,7 @@
         <v>22</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>28</v>
@@ -2118,7 +2086,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>7</v>
       </c>
@@ -2126,7 +2094,7 @@
         <v>22</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>28</v>
@@ -2134,7 +2102,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>7</v>
       </c>
@@ -2142,7 +2110,7 @@
         <v>22</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>28</v>
@@ -2150,7 +2118,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>7</v>
       </c>
@@ -2158,7 +2126,7 @@
         <v>22</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>28</v>
@@ -2166,7 +2134,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>7</v>
       </c>
@@ -2174,7 +2142,7 @@
         <v>22</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>28</v>
@@ -2182,7 +2150,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>7</v>
       </c>
@@ -2190,7 +2158,7 @@
         <v>22</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>28</v>
@@ -2198,7 +2166,7 @@
       <c r="E68" s="6"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>7</v>
       </c>
@@ -2206,7 +2174,7 @@
         <v>22</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>4</v>
@@ -2214,7 +2182,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>7</v>
       </c>
@@ -2222,17 +2190,17 @@
         <v>22</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E70" s="6"/>
       <c r="F70" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>7</v>
       </c>
@@ -2240,17 +2208,17 @@
         <v>22</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>7</v>
       </c>
@@ -2258,17 +2226,17 @@
         <v>22</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>7</v>
       </c>
@@ -2276,17 +2244,17 @@
         <v>22</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E73" s="6"/>
       <c r="F73" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>7</v>
       </c>
@@ -2294,17 +2262,17 @@
         <v>22</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>7</v>
       </c>
@@ -2312,17 +2280,17 @@
         <v>22</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E75" s="6"/>
       <c r="F75" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>7</v>
       </c>
@@ -2330,17 +2298,17 @@
         <v>22</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E76" s="6"/>
       <c r="F76" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>7</v>
       </c>
@@ -2348,17 +2316,17 @@
         <v>22</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E77" s="6"/>
       <c r="F77" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>7</v>
       </c>
@@ -2366,17 +2334,17 @@
         <v>22</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>7</v>
       </c>
@@ -2384,17 +2352,17 @@
         <v>22</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E79" s="6"/>
       <c r="F79" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>7</v>
       </c>
@@ -2402,17 +2370,17 @@
         <v>22</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E80" s="6"/>
       <c r="F80" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>7</v>
       </c>
@@ -2420,17 +2388,17 @@
         <v>22</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E81" s="6"/>
       <c r="F81" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>7</v>
       </c>
@@ -2438,17 +2406,17 @@
         <v>22</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>7</v>
       </c>
@@ -2456,47 +2424,49 @@
         <v>22</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E83" s="6"/>
       <c r="F83" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D84" s="5"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="E84" s="5"/>
-      <c r="F84" s="6"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
-      <c r="F85" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="1:6" ht="14.85" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>15</v>
       </c>
@@ -2504,18 +2474,18 @@
         <v>70</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="6"/>
       <c r="F86" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F84" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F85"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D76:D1048576 D1:D74">
+  <conditionalFormatting sqref="D1:D74 D76:D1048576">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"metr"</formula>
     </cfRule>
@@ -2532,29 +2502,29 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>